<commit_message>
fix(excel), #35: Update logic to parse named ranges.
</commit_message>
<xml_diff>
--- a/test/test_files/test.xlsx
+++ b/test/test_files/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59DCFEE-3E43-AB4E-AC67-C31CC64343D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1971530-CACB-F341-A1BF-85AB0D7ED820}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19300" tabRatio="770" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATH &amp; TRIG" sheetId="3" r:id="rId1"/>
@@ -36,12 +36,16 @@
     <definedName name="e">CORE!$D$4:$E$5</definedName>
     <definedName name="f">CORE!$G$2:$H$5</definedName>
     <definedName name="g">REF!$B$2:$B$5</definedName>
+    <definedName name="h">CORE!$K$4:$K$6 CORE!$J$5:$L$5</definedName>
+    <definedName name="i">SUM(CORE!$M$4:$N$5,h)</definedName>
+    <definedName name="l">h+i</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -1454,14 +1458,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
-    <numFmt numFmtId="8" formatCode="&quot;€&quot;#,##0.00;[Red]\-&quot;€&quot;#,##0.00"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.00000000000000"/>
-    <numFmt numFmtId="166" formatCode="0.000000000000000000"/>
-    <numFmt numFmtId="167" formatCode="0.0000000000000000"/>
-    <numFmt numFmtId="168" formatCode="0.0000000000000000000"/>
-    <numFmt numFmtId="169" formatCode="0.0000000000000000000000"/>
-    <numFmt numFmtId="170" formatCode="&quot;€&quot;#,##0.00000;[Red]\-&quot;€&quot;#,##0.00000"/>
+    <numFmt numFmtId="164" formatCode="&quot;€&quot;#,##0.00;[Red]\-&quot;€&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="167" formatCode="0.000000000000000000"/>
+    <numFmt numFmtId="168" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="169" formatCode="0.0000000000000000000"/>
+    <numFmt numFmtId="170" formatCode="0.0000000000000000000000"/>
+    <numFmt numFmtId="171" formatCode="&quot;€&quot;#,##0.00000;[Red]\-&quot;€&quot;#,##0.00000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1567,14 +1571,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1592,10 +1596,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1608,28 +1612,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -12453,7 +12457,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:AT81">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:AT81">
     <sortCondition ref="A3"/>
   </sortState>
   <mergeCells count="8">
@@ -12510,7 +12514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AV81"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -20456,7 +20460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AV113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -25679,53 +25683,68 @@
         <v>1</v>
       </c>
       <c r="AG7" s="6" t="b">
-        <f t="array" ref="AG7:AV7">ISERR(B7:P7)</f>
-        <v>0</v>
+        <f t="shared" ref="AG7:AV7" si="1">ISERR(B7:P7)</f>
+        <v>1</v>
       </c>
       <c r="AH7" s="6" t="b">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AI7" s="6" t="b">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AJ7" s="6" t="b">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AK7" s="6" t="b">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AL7" s="6" t="b">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AM7" s="6" t="b">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AN7" s="6" t="b">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AO7" s="6" t="b">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AP7" s="6" t="b">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="AQ7" s="6" t="b">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AR7" s="6" t="b">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AS7" s="6" t="b">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AT7" s="6" t="b">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AU7" s="6" t="b">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AV7" s="4" t="b">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.15">
@@ -25776,63 +25795,63 @@
         <v>#REF!</v>
       </c>
       <c r="Q8" s="6" t="b">
-        <f t="shared" ref="Q8:AE8" si="1">ISERROR(B8)</f>
+        <f t="shared" ref="Q8:AE8" si="2">ISERROR(B8)</f>
         <v>0</v>
       </c>
       <c r="R8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="S8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="T8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="V8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="W8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Z8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AA8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AB8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AC8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AD8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AE8" s="6" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AF8" s="6" t="b">
@@ -25840,52 +25859,67 @@
         <v>1</v>
       </c>
       <c r="AG8" s="6" t="b">
-        <f t="array" ref="AG8:AV8">ISERROR(B8:P8)</f>
-        <v>0</v>
+        <f t="shared" ref="AG8:AV8" si="3">ISERROR(B8:P8)</f>
+        <v>1</v>
       </c>
       <c r="AH8" s="6" t="b">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AI8" s="6" t="b">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AJ8" s="6" t="b">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AK8" s="6" t="b">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AL8" s="6" t="b">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AM8" s="6" t="b">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AN8" s="6" t="b">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AO8" s="6" t="b">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AP8" s="6" t="b">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AQ8" s="6" t="b">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AR8" s="6" t="b">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AS8" s="6" t="b">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AT8" s="6" t="b">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AU8" s="6" t="b">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AV8" s="4" t="b">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -31975,39 +32009,39 @@
         <v>58</v>
       </c>
       <c r="W58" s="6">
-        <f t="shared" ref="W58:W59" si="22">ROW(H58)</f>
+        <f>ROW(H58)</f>
         <v>58</v>
       </c>
       <c r="X58" s="6">
-        <f t="shared" ref="X58:X59" si="23">ROW(I58)</f>
+        <f t="shared" ref="X58:X59" si="22">ROW(I58)</f>
         <v>58</v>
       </c>
       <c r="Y58" s="6">
-        <f t="shared" ref="Y58:Y59" si="24">ROW(J58)</f>
+        <f t="shared" ref="Y58:Y59" si="23">ROW(J58)</f>
         <v>58</v>
       </c>
       <c r="Z58" s="6">
-        <f t="shared" ref="Z58:Z59" si="25">ROW(K58)</f>
+        <f t="shared" ref="Z58:Z59" si="24">ROW(K58)</f>
         <v>58</v>
       </c>
       <c r="AA58" s="6">
-        <f t="shared" ref="AA58:AA59" si="26">ROW(L58)</f>
+        <f t="shared" ref="AA58:AA59" si="25">ROW(L58)</f>
         <v>58</v>
       </c>
       <c r="AB58" s="6">
-        <f t="shared" ref="AB58:AB59" si="27">ROW(M58)</f>
+        <f t="shared" ref="AB58:AB59" si="26">ROW(M58)</f>
         <v>58</v>
       </c>
       <c r="AC58" s="6">
-        <f t="shared" ref="AC58:AC59" si="28">ROW(N58)</f>
+        <f t="shared" ref="AC58:AC59" si="27">ROW(N58)</f>
         <v>58</v>
       </c>
       <c r="AD58" s="6">
-        <f t="shared" ref="AD58:AD59" si="29">ROW(O58)</f>
+        <f t="shared" ref="AD58:AD59" si="28">ROW(O58)</f>
         <v>58</v>
       </c>
       <c r="AE58" s="6">
-        <f t="shared" ref="AE58:AE59" si="30">ROW(P58)</f>
+        <f t="shared" ref="AE58:AE59" si="29">ROW(P58)</f>
         <v>58</v>
       </c>
       <c r="AF58" s="4" t="e">
@@ -32105,39 +32139,39 @@
         <v>59</v>
       </c>
       <c r="W59" s="6">
+        <f t="shared" ref="W58:W59" si="30">ROW(H59)</f>
+        <v>59</v>
+      </c>
+      <c r="X59" s="6">
         <f t="shared" si="22"/>
         <v>59</v>
       </c>
-      <c r="X59" s="6">
+      <c r="Y59" s="6">
         <f t="shared" si="23"/>
         <v>59</v>
       </c>
-      <c r="Y59" s="6">
+      <c r="Z59" s="6">
         <f t="shared" si="24"/>
         <v>59</v>
       </c>
-      <c r="Z59" s="6">
+      <c r="AA59" s="6">
         <f t="shared" si="25"/>
         <v>59</v>
       </c>
-      <c r="AA59" s="6">
+      <c r="AB59" s="6">
         <f t="shared" si="26"/>
         <v>59</v>
       </c>
-      <c r="AB59" s="6">
+      <c r="AC59" s="6">
         <f t="shared" si="27"/>
         <v>59</v>
       </c>
-      <c r="AC59" s="6">
+      <c r="AD59" s="6">
         <f t="shared" si="28"/>
         <v>59</v>
       </c>
-      <c r="AD59" s="6">
+      <c r="AE59" s="6">
         <f t="shared" si="29"/>
-        <v>59</v>
-      </c>
-      <c r="AE59" s="6">
-        <f t="shared" si="30"/>
         <v>59</v>
       </c>
       <c r="AF59" s="4">
@@ -34487,6 +34521,9 @@
       <c r="E4">
         <v>4</v>
       </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
       <c r="G4">
         <v>5</v>
       </c>
@@ -34507,6 +34544,14 @@
       <c r="N4">
         <v>2</v>
       </c>
+      <c r="Q4">
+        <f>h</f>
+        <v>5</v>
+      </c>
+      <c r="R4">
+        <f>i</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5">
@@ -34538,6 +34583,14 @@
       </c>
       <c r="N5">
         <v>2</v>
+      </c>
+      <c r="Q5">
+        <f>h</f>
+        <v>5</v>
+      </c>
+      <c r="R5">
+        <f>l</f>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.2">
@@ -34621,11 +34674,11 @@
       </c>
       <c r="D9">
         <f>SUM(B2:E5:f)</f>
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E9">
         <f ca="1">C9+D9+G7+G2+F1+F9</f>
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F9">
         <f ca="1">SUM(INDIRECT("f"))</f>

</xml_diff>